<commit_message>
Auto stash before merge of "master" and "HenryNebula/master"
</commit_message>
<xml_diff>
--- a/report/工作簿1.xlsx
+++ b/report/工作簿1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HenryHuang/Desktop/DataMining/diff_privacy_test/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E42D610-977A-4E42-BDCD-35025B2A7E88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3B2F47-E887-2A4F-86C6-ED40AA022FAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{55EF4ED7-F4C1-E742-930A-2D80BBA49619}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
   <si>
     <t>loc=6528</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +78,18 @@
     <t>loc=2500</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve">sum of posterior </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spatial coverage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>our model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -122,9 +134,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7569,13 +7584,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0708E5F8-089D-694F-AFB0-7DA93AA78C02}">
-  <dimension ref="O5:T79"/>
+  <dimension ref="N5:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M6" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="L84" workbookViewId="0">
+      <selection activeCell="S105" sqref="S105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="15" max="15" width="19.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5" spans="15:20">
       <c r="P5" t="s">
@@ -8191,7 +8209,69 @@
         <v>13344</v>
       </c>
     </row>
+    <row r="99" spans="14:17">
+      <c r="O99" t="s">
+        <v>14</v>
+      </c>
+      <c r="P99" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="14:17">
+      <c r="N100" t="s">
+        <v>4</v>
+      </c>
+      <c r="O100">
+        <v>935</v>
+      </c>
+      <c r="P100" s="1">
+        <v>425.26</v>
+      </c>
+      <c r="Q100" s="1"/>
+    </row>
+    <row r="101" spans="14:17">
+      <c r="N101" t="s">
+        <v>15</v>
+      </c>
+      <c r="O101">
+        <v>563</v>
+      </c>
+      <c r="P101" s="1">
+        <v>380.27</v>
+      </c>
+      <c r="Q101" s="1"/>
+    </row>
+    <row r="102" spans="14:17">
+      <c r="N102" t="s">
+        <v>6</v>
+      </c>
+      <c r="O102">
+        <v>549</v>
+      </c>
+      <c r="P102" s="1">
+        <v>423.87</v>
+      </c>
+      <c r="Q102" s="1"/>
+    </row>
+    <row r="103" spans="14:17">
+      <c r="N103" t="s">
+        <v>7</v>
+      </c>
+      <c r="O103">
+        <v>534</v>
+      </c>
+      <c r="P103" s="1">
+        <v>427.56</v>
+      </c>
+      <c r="Q103" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="P100:Q100"/>
+    <mergeCell ref="P101:Q101"/>
+    <mergeCell ref="P102:Q102"/>
+    <mergeCell ref="P103:Q103"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Big change on Posterior is coming
</commit_message>
<xml_diff>
--- a/report/工作簿1.xlsx
+++ b/report/工作簿1.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HenryHuang/Desktop/DataMining/diff_privacy_test/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3B2F47-E887-2A4F-86C6-ED40AA022FAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6423B8F-55B3-8B4F-A2A5-3BADD976ADB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" xr2:uid="{55EF4ED7-F4C1-E742-930A-2D80BBA49619}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$O$123</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$P$122:$T$122</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$P$123:$T$123</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$O$123</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$P$122:$T$122</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$P$123:$T$123</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
   <si>
     <t>loc=6528</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,12 +98,36 @@
     <t>our model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>RAPPOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>target=609, #candidate=40, k=5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>target=165, #candidate=20, k=5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p=1e-6, our alg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p=1e-3, our alg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Relative Performance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,6 +140,14 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -134,12 +174,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3808,6 +3854,906 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$123</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>target=165, #candidate=20, k=5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$P$122:$T$122</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>no-noise</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>our-algorithm</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RAPPOR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>noisy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$123:$T$123</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-63B7-9646-B6C4-6E9E88744AC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1558208448"/>
+        <c:axId val="1552244944"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1558208448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1552244944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1552244944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1558208448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>target=158, #candidate=20, k=5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$130</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>target=609, #candidate=40, k=5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$P$129:$T$129</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>no-noise</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>our-algorithm</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>RAPPOR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>noisy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$130:$T$130</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3752-C740-BF20-E7DF1F9CD5F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1559607568"/>
+        <c:axId val="1559609248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1559607568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1559609248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1559609248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1559607568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Relative Performance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$P$132:$S$132</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>no-noise</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>p=1e-6, our alg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>p=1e-3, our alg</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$133:$S$133</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.8169999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3640000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B01C-684F-AE5E-F03AABE0AC3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1560118640"/>
+        <c:axId val="1560120320"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1560118640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1560120320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1560120320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1560118640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4048,6 +4994,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6564,6 +7630,1515 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7284,6 +9859,114 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB0B00F6-F43D-E440-AC53-9EB3004EC983}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1377950</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="图表 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{233D8E80-C667-9F44-A584-D5DB9FB20965}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>768350</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="图表 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C00DB454-7C12-C349-8931-17691C63285D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7584,15 +10267,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0708E5F8-089D-694F-AFB0-7DA93AA78C02}">
-  <dimension ref="N5:T103"/>
+  <dimension ref="N5:T136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L84" workbookViewId="0">
-      <selection activeCell="S105" sqref="S105"/>
+    <sheetView tabSelected="1" topLeftCell="J112" workbookViewId="0">
+      <selection activeCell="T136" sqref="T136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="15" max="15" width="19.83203125" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="15:20">
@@ -8224,10 +10908,10 @@
       <c r="O100">
         <v>935</v>
       </c>
-      <c r="P100" s="1">
+      <c r="P100" s="2">
         <v>425.26</v>
       </c>
-      <c r="Q100" s="1"/>
+      <c r="Q100" s="2"/>
     </row>
     <row r="101" spans="14:17">
       <c r="N101" t="s">
@@ -8236,10 +10920,10 @@
       <c r="O101">
         <v>563</v>
       </c>
-      <c r="P101" s="1">
+      <c r="P101" s="2">
         <v>380.27</v>
       </c>
-      <c r="Q101" s="1"/>
+      <c r="Q101" s="2"/>
     </row>
     <row r="102" spans="14:17">
       <c r="N102" t="s">
@@ -8248,10 +10932,10 @@
       <c r="O102">
         <v>549</v>
       </c>
-      <c r="P102" s="1">
+      <c r="P102" s="2">
         <v>423.87</v>
       </c>
-      <c r="Q102" s="1"/>
+      <c r="Q102" s="2"/>
     </row>
     <row r="103" spans="14:17">
       <c r="N103" t="s">
@@ -8260,10 +10944,155 @@
       <c r="O103">
         <v>534</v>
       </c>
-      <c r="P103" s="1">
+      <c r="P103" s="2">
         <v>427.56</v>
       </c>
-      <c r="Q103" s="1"/>
+      <c r="Q103" s="2"/>
+    </row>
+    <row r="122" spans="15:20">
+      <c r="O122" s="1"/>
+      <c r="P122" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S122" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T122" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="15:20">
+      <c r="O123" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P123" s="1">
+        <v>2.79</v>
+      </c>
+      <c r="Q123" s="1">
+        <v>1.68</v>
+      </c>
+      <c r="R123" s="1">
+        <v>1.36</v>
+      </c>
+      <c r="S123" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="T123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="15:20">
+      <c r="O124" s="1"/>
+      <c r="P124" s="1"/>
+      <c r="Q124" s="1"/>
+      <c r="R124" s="1"/>
+      <c r="S124" s="1"/>
+      <c r="T124" s="1"/>
+    </row>
+    <row r="125" spans="15:20">
+      <c r="O125" s="1"/>
+      <c r="P125" s="1"/>
+      <c r="Q125" s="1"/>
+      <c r="R125" s="1"/>
+      <c r="S125" s="1"/>
+      <c r="T125" s="1"/>
+    </row>
+    <row r="126" spans="15:20">
+      <c r="O126" s="1"/>
+      <c r="P126" s="1"/>
+      <c r="Q126" s="1"/>
+      <c r="R126" s="1"/>
+      <c r="S126" s="1"/>
+      <c r="T126" s="1"/>
+    </row>
+    <row r="129" spans="15:20">
+      <c r="O129" s="1"/>
+      <c r="P129" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q129" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S129" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T129" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="15:20" ht="35">
+      <c r="O130" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P130" s="3">
+        <v>1.81</v>
+      </c>
+      <c r="Q130" s="1">
+        <v>1.27</v>
+      </c>
+      <c r="R130" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="S130" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="T130" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="15:20">
+      <c r="P132" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>19</v>
+      </c>
+      <c r="R132" t="s">
+        <v>20</v>
+      </c>
+      <c r="S132" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="15:20">
+      <c r="O133" t="s">
+        <v>21</v>
+      </c>
+      <c r="P133">
+        <v>1.8169999999999999</v>
+      </c>
+      <c r="Q133">
+        <v>1.75</v>
+      </c>
+      <c r="R133">
+        <v>1.3640000000000001</v>
+      </c>
+      <c r="S133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="15:20">
+      <c r="P136">
+        <v>2086</v>
+      </c>
+      <c r="Q136">
+        <v>2010</v>
+      </c>
+      <c r="R136">
+        <v>1566</v>
+      </c>
+      <c r="S136">
+        <v>1148</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>